<commit_message>
added aggregate info for sean
</commit_message>
<xml_diff>
--- a/figures/Results.xlsx
+++ b/figures/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Random Forest</t>
   </si>
@@ -73,12 +73,48 @@
   <si>
     <t>Threshold</t>
   </si>
+  <si>
+    <t>k-Means</t>
+  </si>
+  <si>
+    <t>w/PCA</t>
+  </si>
+  <si>
+    <t>w/o PCA</t>
+  </si>
+  <si>
+    <t>1-NN</t>
+  </si>
+  <si>
+    <t>&lt;-- super slow when not using PCA</t>
+  </si>
+  <si>
+    <t>3-NN</t>
+  </si>
+  <si>
+    <t>5-NN</t>
+  </si>
+  <si>
+    <t>7-NN</t>
+  </si>
+  <si>
+    <t>&lt;-- super super super slow</t>
+  </si>
+  <si>
+    <t>Bagged Decision Tree</t>
+  </si>
+  <si>
+    <t>Boosted Decision Tree</t>
+  </si>
+  <si>
+    <t>Analysis for Sean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,16 +122,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -103,14 +175,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -171,7 +298,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -405,11 +531,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="187520344"/>
-        <c:axId val="187520736"/>
+        <c:axId val="524680680"/>
+        <c:axId val="524681072"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="187520344"/>
+        <c:axId val="524680680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -441,7 +567,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -508,7 +633,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187520736"/>
+        <c:crossAx val="524681072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -517,7 +642,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="187520736"/>
+        <c:axId val="524681072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -565,7 +690,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -626,7 +750,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187520344"/>
+        <c:crossAx val="524680680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -640,7 +764,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -747,7 +870,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -981,11 +1103,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="187523480"/>
-        <c:axId val="187521128"/>
+        <c:axId val="524671272"/>
+        <c:axId val="524671664"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="187523480"/>
+        <c:axId val="524671272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,7 +1139,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1084,7 +1205,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187521128"/>
+        <c:crossAx val="524671664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -1093,7 +1214,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="187521128"/>
+        <c:axId val="524671664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1141,7 +1262,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1202,7 +1322,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187523480"/>
+        <c:crossAx val="524671272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1216,7 +1336,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1323,7 +1442,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1504,11 +1622,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="452504600"/>
-        <c:axId val="452508128"/>
+        <c:axId val="524676368"/>
+        <c:axId val="524681464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="452504600"/>
+        <c:axId val="524676368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1540,7 +1658,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1607,7 +1724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="452508128"/>
+        <c:crossAx val="524681464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1615,7 +1732,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="452508128"/>
+        <c:axId val="524681464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1663,7 +1780,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1724,7 +1840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="452504600"/>
+        <c:crossAx val="524676368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1738,7 +1854,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1845,7 +1960,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2052,11 +2166,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="532123224"/>
-        <c:axId val="532121656"/>
+        <c:axId val="524672448"/>
+        <c:axId val="524675584"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="532123224"/>
+        <c:axId val="524672448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2093,7 +2207,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2160,7 +2273,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="532121656"/>
+        <c:crossAx val="524675584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -2169,7 +2282,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="532121656"/>
+        <c:axId val="524675584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2217,7 +2330,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2278,7 +2390,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="532123224"/>
+        <c:crossAx val="524672448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2292,7 +2404,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2399,7 +2510,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2543,8 +2653,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="533153960"/>
-        <c:axId val="547092064"/>
+        <c:axId val="524683816"/>
+        <c:axId val="524684600"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -2615,11 +2725,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="627125824"/>
-        <c:axId val="531591248"/>
+        <c:axId val="524685384"/>
+        <c:axId val="524684992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="533153960"/>
+        <c:axId val="524683816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2653,7 +2763,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2720,13 +2829,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="547092064"/>
+        <c:crossAx val="524684600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="7"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="547092064"/>
+        <c:axId val="524684600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2774,7 +2883,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2835,12 +2943,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533153960"/>
+        <c:crossAx val="524683816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="531591248"/>
+        <c:axId val="524684992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2879,12 +2987,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627125824"/>
+        <c:crossAx val="524685384"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="627125824"/>
+        <c:axId val="524685384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2894,7 +3002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="531591248"/>
+        <c:crossAx val="524684992"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2908,7 +3016,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3159,8 +3266,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="533151608"/>
-        <c:axId val="533152000"/>
+        <c:axId val="558765192"/>
+        <c:axId val="558766368"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -3231,11 +3338,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="453387104"/>
-        <c:axId val="453387496"/>
+        <c:axId val="558766760"/>
+        <c:axId val="558767152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="533151608"/>
+        <c:axId val="558765192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3336,13 +3443,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533152000"/>
+        <c:crossAx val="558766368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="7"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="533152000"/>
+        <c:axId val="558766368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3451,12 +3558,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533151608"/>
+        <c:crossAx val="558765192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="453387496"/>
+        <c:axId val="558767152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3495,12 +3602,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453387104"/>
+        <c:crossAx val="558766760"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="453387104"/>
+        <c:axId val="558766760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3510,7 +3617,617 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="453387496"/>
+        <c:crossAx val="558767152"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy of k-Means Classifer</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$114</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>with PCA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$113:$H$113</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$114:$H$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>51.225099999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58.296300000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.965499999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.744399999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60.508600000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58.585799999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="558767936"/>
+        <c:axId val="558765584"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$115</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>without PCA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$118:$B$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$118:$C$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>57.882800000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.882800000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="558760880"/>
+        <c:axId val="558765976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="558767936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PCA Dimensions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="558765584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="7"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="558765584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Accuracy (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="558767936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="558765976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="558760880"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="558760880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="558765976"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3831,6 +4548,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -6399,6 +7156,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7104,6 +8377,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7370,10 +8675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I92" sqref="I92"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7826,7 +9131,7 @@
         <v>96.33</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B97">
         <v>100</v>
       </c>
@@ -7835,7 +9140,239 @@
         <v>96.33</v>
       </c>
     </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>12</v>
+      </c>
+      <c r="B113">
+        <v>2</v>
+      </c>
+      <c r="C113">
+        <v>3</v>
+      </c>
+      <c r="D113">
+        <v>5</v>
+      </c>
+      <c r="E113">
+        <v>10</v>
+      </c>
+      <c r="F113">
+        <v>25</v>
+      </c>
+      <c r="G113">
+        <v>50</v>
+      </c>
+      <c r="H113">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <v>51.225099999999998</v>
+      </c>
+      <c r="D114">
+        <v>58.296300000000002</v>
+      </c>
+      <c r="E114">
+        <v>57.965499999999999</v>
+      </c>
+      <c r="F114">
+        <v>63.744399999999999</v>
+      </c>
+      <c r="G114">
+        <v>60.508600000000001</v>
+      </c>
+      <c r="H114">
+        <v>58.585799999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115">
+        <v>57.882800000000003</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C117" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <f>B115</f>
+        <v>57.882800000000003</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B119">
+        <v>100</v>
+      </c>
+      <c r="C119">
+        <f>B115</f>
+        <v>57.882800000000003</v>
+      </c>
+    </row>
+    <row r="129" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="131" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C131" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B132" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C132" s="2">
+        <v>91.97</v>
+      </c>
+      <c r="D132" s="2">
+        <v>96.31</v>
+      </c>
+    </row>
+    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B133" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C133" s="2">
+        <v>93.99</v>
+      </c>
+      <c r="D133" s="2">
+        <v>93.54</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F133" s="8"/>
+      <c r="G133" s="8"/>
+      <c r="H133" s="8"/>
+      <c r="I133" s="8"/>
+    </row>
+    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B134" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C134" s="2">
+        <v>93.03</v>
+      </c>
+      <c r="D134" s="2">
+        <v>92.18</v>
+      </c>
+      <c r="E134" s="3"/>
+      <c r="F134" s="8"/>
+      <c r="G134" s="8"/>
+      <c r="H134" s="8"/>
+      <c r="I134" s="8"/>
+    </row>
+    <row r="135" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B135" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C135" s="2">
+        <v>92.58</v>
+      </c>
+      <c r="D135" s="2">
+        <v>91.65</v>
+      </c>
+      <c r="E135" s="3"/>
+      <c r="F135" s="8"/>
+      <c r="G135" s="8"/>
+      <c r="H135" s="8"/>
+      <c r="I135" s="8"/>
+    </row>
+    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B136" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C136" s="2">
+        <v>91.68</v>
+      </c>
+      <c r="D136" s="2">
+        <v>91.08</v>
+      </c>
+      <c r="E136" s="3"/>
+      <c r="F136" s="8"/>
+      <c r="G136" s="8"/>
+      <c r="H136" s="8"/>
+      <c r="I136" s="8"/>
+    </row>
+    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B137" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C137" s="4">
+        <v>52.34</v>
+      </c>
+      <c r="D137" s="5">
+        <v>96.33</v>
+      </c>
+      <c r="E137" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B138" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C138" s="6">
+        <v>74.31</v>
+      </c>
+      <c r="D138" s="6">
+        <v>75.7</v>
+      </c>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B139" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C139" s="6">
+        <v>74.42</v>
+      </c>
+      <c r="D139" s="6">
+        <v>77.03</v>
+      </c>
+    </row>
+    <row r="140" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B140" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C140" s="6">
+        <v>84.87</v>
+      </c>
+      <c r="D140" s="7"/>
+    </row>
+    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B141" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C141" s="6">
+        <v>74.98</v>
+      </c>
+      <c r="D141" s="7"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E133:I136"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>